<commit_message>
CourseWorks with OoPaEM 3Lab
</commit_message>
<xml_diff>
--- a/4-1 labs.xlsx
+++ b/4-1 labs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSTU\4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSTU\4\4-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDC2F22-E183-4027-B0D0-33A2C65420F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50832F3-BC68-44C4-B6F9-7675E5678624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Предметы</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Защита</t>
+  </si>
+  <si>
+    <t>Конец (Проект)</t>
   </si>
 </sst>
 </file>
@@ -116,7 +119,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -132,12 +135,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -276,22 +273,22 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -577,12 +574,13 @@
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="13" max="13" width="15.5546875" customWidth="1"/>
     <col min="17" max="17" width="13.33203125" customWidth="1"/>
     <col min="18" max="18" width="10.77734375" customWidth="1"/>
   </cols>
@@ -647,7 +645,7 @@
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="26"/>
+      <c r="B2" s="25"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -671,7 +669,7 @@
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="25"/>
+      <c r="B3" s="24"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -694,7 +692,7 @@
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="24"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -704,10 +702,10 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
-      <c r="L4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="M4" s="7"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="28" t="s">
+        <v>14</v>
+      </c>
       <c r="N4" s="8"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -721,7 +719,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="28" t="s">
+      <c r="I5" s="27" t="s">
         <v>2</v>
       </c>
       <c r="J5" s="7"/>
@@ -739,7 +737,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
-      <c r="I6" s="27" t="s">
+      <c r="I6" s="26" t="s">
         <v>4</v>
       </c>
     </row>
@@ -748,7 +746,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="23"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="15"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -777,7 +775,7 @@
       </c>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="26" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="19"/>

</xml_diff>